<commit_message>
Added commute time info
</commit_message>
<xml_diff>
--- a/data/EarlyVotingTimes.xlsx
+++ b/data/EarlyVotingTimes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sharon\My Documents Data Drive\R\EarlyVoting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{89081984-B4A2-41BB-969E-153132EAEF0D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{371244E0-CCEA-4F36-80D6-11BA93FBE978}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8865" firstSheet="16" activeTab="21" xr2:uid="{8180FAB9-CEFF-476A-A9D7-1FD06D90AD4E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8865" firstSheet="19" activeTab="24" xr2:uid="{8180FAB9-CEFF-476A-A9D7-1FD06D90AD4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Plymouth" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,9 @@
     <sheet name="Springfield" sheetId="20" r:id="rId20"/>
     <sheet name="Lowell" sheetId="21" r:id="rId21"/>
     <sheet name="Hudson" sheetId="22" r:id="rId22"/>
+    <sheet name="Natick" sheetId="23" r:id="rId23"/>
+    <sheet name="Arlington" sheetId="24" r:id="rId24"/>
+    <sheet name="Southborough" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1657" uniqueCount="206">
   <si>
     <t>Day</t>
   </si>
@@ -643,6 +646,27 @@
   </si>
   <si>
     <t>78 MAIN STREET HUDSON, MA. 01749</t>
+  </si>
+  <si>
+    <t>NATICK TOWN HALL</t>
+  </si>
+  <si>
+    <t>13 EAST CENTRAL ST.</t>
+  </si>
+  <si>
+    <t>TOWN HALL AUDITORIUM</t>
+  </si>
+  <si>
+    <t>730 MASSACHUSETTS AVENUE</t>
+  </si>
+  <si>
+    <t>SOUTHBOROUGH TOWN HOUSE</t>
+  </si>
+  <si>
+    <t>17 COMMON STREET SOUTHBOROUGH, MA 01772</t>
+  </si>
+  <si>
+    <t>8:00 AM - 6:00 PM</t>
   </si>
 </sst>
 </file>
@@ -5648,7 +5672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C01D5EC-9EAE-4370-BBB2-C440E8B25F23}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
@@ -5856,6 +5880,649 @@
       </c>
       <c r="E12" t="s">
         <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C98FE8-A2C2-4D19-BAB8-5A856A598352}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43395</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43396</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43397</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43398</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43399</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43402</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43403</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43404</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43405</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43406</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D690C914-D4AE-40D7-81FE-722A97A4628C}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43395</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43396</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43397</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43398</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43399</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43402</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43403</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43404</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43405</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>201</v>
+      </c>
+      <c r="E10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43406</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3779A7D9-440D-49BA-AC87-F107E7283642}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43395</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43396</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43397</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43398</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43399</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43402</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43403</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43404</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43405</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43406</v>
+      </c>
+      <c r="C12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>